<commit_message>
added tables for learn/classify
</commit_message>
<xml_diff>
--- a/thesis/data/Review of Learning & Classification.xlsx
+++ b/thesis/data/Review of Learning & Classification.xlsx
@@ -326,51 +326,6 @@
   <si>
     <t>Ricordeau (2003) and 
 Ricordeau and Liquiere (2007)</t>
-  </si>
-  <si>
-    <t>used FCA to generalize policies in reinforcement learning by grouping similar states using their descriptions.
-%\\2003 paper
-\\One of the very interesting properties of Reinforcement Learning algorithms is that they allow learning without prior knowledge of the environment. However, when the agents use algorithms that enable a generalization of the learning, they are unable to explain their choices. Neural networks are good examples of this problem. After a reminder about the basis of Reinforcement Learning, the Lattice Concept will be introduced. Then,
-Q-Concept-Learning, a Reinforcement Learning algorithm that enables a generalization of the learning, the use of structured languages as well as an explanation of the agent’s choices will be presented.
-\begin{comment}
-\\First, we exposed the basis of Reinforcement Learning and concept lattice. We explained how to use concept lattice to structure the memory of an agent which
-learns with reinforcement and the algorithmic consequences.
-\\The first advantage of this method is the possibility of using more structured languages than attributes-value languages to describe the environment of the agent, using the Learning-Languages (Liqui`ere M. (2002) [4]).
-\\Then, we presented Q-Concept-Learning, a Reinforcement Learning algorithm which allows generalizing the learning, i.e. to use previously learned knowledge on new situations. This algorithm keeps the symbolic representation, contrary to other generalization
-methods like approximation function or neural networks. Moreover, Q-Concept-Learning allows building a part of the model of the agent’s environment. It can return the useful concepts for the task it learned. We implemented Q-Concept-Learning on a simple
-example which permitted to show the improvement due to generalization as well as the return of the useful concepts.
-%\\2007
-\\The generalization of policies in reinforcement learning is a
-main issue, both from the theoretical model point of view and for their
-applicability. However, generalizing from a set of examples or searching
-for regularities is a problem which has already been intensively studied
-in machine learning. Our work uses techniques in which generalizations
-are constrained by a language bias, in order to regroup similar states.
-Such generalizations are principally based on the properties of concept
-lattices. To guide the possible groupings of similar environment’s states,
-we propose a general algebraic framework, considering the generalization
-of policies through a set partition of the states and using a language bias
-as an a priori knowledge. We give an application as an example of our
-approach by proposing and experimenting a bottom-up algorithm.
-\\First, we reminded the reader of the general principles in the use of a Galois lattice as a generalization space for a set of objects described with a generalization
-language. Then, we extended these results to define an original generalization
-space for the partitions instead of powerset, in particular by introducing the
-notion of partition agreeing with a language. We showed that, considering generalization as a partitioning, this structure can be used to generalize learning
-in reinforcement learning. Finally, we proposed a bottom-up algorithm which
-through a reinforcement learning and a generalization language made it possible
-to produce general rules linking description elements of the environment and
-optimal actions.
-This work considered principally the algebraical aspects. Consequently, we didn’t
-treat two remaining important issues: “How to use the rules on unknown examples” and “How to deal with knowledge uncertainty”.
-Our future work will focus on three directions. First, a more formal link between
-our work and the relational reinforcement learning [9]. Secondly, an algorithmic improvement, studying the different ways of exploring the space search and
-the classical balancing between spatial and temporal complexity. Thirdly, we
-will consider the exploration-exploitation problem, i.e. using previously acquired
-knowledge or acquiring new knowledge and as a corollary, managing knowledge
-uncertainty. It remains a difficult problem in machine learning and in reinforcement learning in particular. In our case, it’s transposed in a particular way as
-the concept reliability, already presented in [10]. We think that a relevant approach can consists in the explicit management of second order elements (states
-distribution, maximal reward,. . . ) directly through the algorithms.
-\end{comment}</t>
   </si>
   <si>
     <t>Aoun-Allah and Mineau (2006)</t>
@@ -788,6 +743,50 @@
 from contextual classi®ers, we may be able to use some techniques (like evidence
 theory) to accumulate the collected evidence. All these eorts may result in the
 improvement of the performance of our algorithms.</t>
+  </si>
+  <si>
+    <t>used FCA to generalize policies in reinforcement learning by grouping similar states using their descriptions.
+%\\2003 paper
+\\One of the very interesting properties of Reinforcement Learning algorithms is that they allow learning without prior knowledge of the environment. However, when the agents use algorithms that enable a generalization of the learning, they are unable to explain their choices. Neural networks are good examples of this problem. After a reminder about the basis of Reinforcement Learning, the Lattice Concept will be introduced. Then,
+Q-Concept-Learning, a Reinforcement Learning algorithm that enables a generalization of the learning, the use of structured languages as well as an explanation of the agent’s choices will be presented.
+\begin{comment}
+\\First, we exposed the basis of Reinforcement Learning and concept lattice. We explained how to use concept lattice to structure the memory of an agent which
+learns with reinforcement and the algorithmic consequences.
+\\The first advantage of this method is the possibility of using more structured languages than attributes-value languages to describe the environment of the agent, using the Learning-Languages (Liqui`ere M. (2002) [4]).
+\\Then, we presented Q-Concept-Learning, a Reinforcement Learning algorithm which allows generalizing the learning, i.e. to use previously learned knowledge on new situations. This algorithm keeps the symbolic representation, contrary to other generalization
+methods like approximation function or neural networks. Moreover, Q-Concept-Learning allows building a part of the model of the agent’s environment. It can return the useful concepts for the task it learned. We implemented Q-Concept-Learning on a simple example which permitted to show the improvement due to generalization as well as the return of the useful concepts.
+%\\2007
+\\The generalization of policies in reinforcement learning is a
+main issue, both from the theoretical model point of view and for their
+applicability. However, generalizing from a set of examples or searching
+for regularities is a problem which has already been intensively studied
+in machine learning. Our work uses techniques in which generalizations
+are constrained by a language bias, in order to regroup similar states.
+Such generalizations are principally based on the properties of concept
+lattices. To guide the possible groupings of similar environment’s states,
+we propose a general algebraic framework, considering the generalization
+of policies through a set partition of the states and using a language bias
+as an a priori knowledge. We give an application as an example of our
+approach by proposing and experimenting a bottom-up algorithm.
+\\First, we reminded the reader of the general principles in the use of a Galois lattice as a generalization space for a set of objects described with a generalization
+language. Then, we extended these results to define an original generalization
+space for the partitions instead of powerset, in particular by introducing the
+notion of partition agreeing with a language. We showed that, considering generalization as a partitioning, this structure can be used to generalize learning
+in reinforcement learning. Finally, we proposed a bottom-up algorithm which
+through a reinforcement learning and a generalization language made it possible
+to produce general rules linking description elements of the environment and
+optimal actions.
+This work considered principally the algebraical aspects. Consequently, we didn’t
+treat two remaining important issues: “How to use the rules on unknown examples” and “How to deal with knowledge uncertainty”.
+Our future work will focus on three directions. First, a more formal link between
+our work and the relational reinforcement learning [9]. Secondly, an algorithmic improvement, studying the different ways of exploring the space search and
+the classical balancing between spatial and temporal complexity. Thirdly, we
+will consider the exploration-exploitation problem, i.e. using previously acquired
+knowledge or acquiring new knowledge and as a corollary, managing knowledge
+uncertainty. It remains a difficult problem in machine learning and in reinforcement learning in particular. In our case, it’s transposed in a particular way as
+the concept reliability, already presented in [10]. We think that a relevant approach can consists in the explicit management of second order elements (states
+distribution, maximal reward,. . . ) directly through the algorithms.
+\end{comment}</t>
   </si>
 </sst>
 </file>
@@ -1123,9 +1122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1133,52 +1130,52 @@
     <col min="2" max="2" width="196.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="360" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="375" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="330" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
@@ -1191,10 +1188,10 @@
     </row>
     <row r="8" spans="1:2" ht="360" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="405" x14ac:dyDescent="0.25">
@@ -1231,10 +1228,10 @@
     </row>
     <row r="13" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
@@ -1242,23 +1239,23 @@
         <v>18</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="360" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="390" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -1287,10 +1284,10 @@
     </row>
     <row r="20" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
@@ -1303,26 +1300,26 @@
     </row>
     <row r="22" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>